<commit_message>
More open format, Integration testing and New Tests
</commit_message>
<xml_diff>
--- a/Assets/TemplateData.xlsx
+++ b/Assets/TemplateData.xlsx
@@ -1,87 +1,108 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="13140" windowWidth="24240" xWindow="-120" yWindow="-120"/>
+    <workbookView windowWidth="24000" windowHeight="9795"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Items" sheetId="1" relationships:id="rId1"/>
-    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Log" sheetId="5" relationships:id="rId2"/>
-    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Report Data" sheetId="3" relationships:id="rId3"/>
-    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Price Log" sheetId="2" relationships:id="rId4"/>
+    <sheet name="Items" sheetId="1" r:id="rId1"/>
+    <sheet name="Report Data" sheetId="3" r:id="rId2"/>
+    <sheet name="Price Log" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>Price</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>Cost</t>
   </si>
   <si>
     <t>Inventory</t>
   </si>
   <si>
-    <t>Cost</t>
+    <t>null</t>
+  </si>
+  <si>
+    <t>The_World</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Trucks_having_sex</t>
+  </si>
+  <si>
+    <t>Retarded</t>
+  </si>
+  <si>
+    <t>Memories</t>
+  </si>
+  <si>
+    <t>Piano_Book</t>
+  </si>
+  <si>
+    <t>verrr</t>
+  </si>
+  <si>
+    <t>rrreee</t>
+  </si>
+  <si>
+    <t>Mixed_Nut_can_2</t>
+  </si>
+  <si>
+    <t>Cracker_Cart</t>
+  </si>
+  <si>
+    <t>Samus</t>
+  </si>
+  <si>
+    <t>rejlk</t>
+  </si>
+  <si>
+    <t>333</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Revenue</t>
   </si>
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Revenue</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>abcdefghijk2</t>
-  </si>
-  <si>
-    <t>Velvet</t>
-  </si>
-  <si>
-    <t>The_World</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Retarded</t>
-  </si>
-  <si>
-    <t>Memories</t>
-  </si>
-  <si>
-    <t>Piano_Book</t>
+    <t>2021/12/1</t>
+  </si>
+  <si>
+    <t>2021/12/2</t>
+  </si>
+  <si>
+    <t>2021/12/3</t>
+  </si>
+  <si>
+    <t>2021/12/4</t>
+  </si>
+  <si>
+    <t>2021/12/5</t>
+  </si>
+  <si>
+    <t>2021/12/6</t>
+  </si>
+  <si>
+    <t>2021/12/30</t>
   </si>
   <si>
     <t>1</t>
@@ -97,115 +118,375 @@
   </si>
   <si>
     <t>Render</t>
-  </si>
-  <si>
-    <t>verrr</t>
-  </si>
-  <si>
-    <t>2021/12/1</t>
-  </si>
-  <si>
-    <t>2021/12/2</t>
-  </si>
-  <si>
-    <t>2021/12/3</t>
-  </si>
-  <si>
-    <t>2021/12/4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="6">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
-    <fill>
-      <patternFill patternType="none">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125">
-        <fgColor/>
-        <bgColor/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor auto="true"/>
-        <bgColor auto="true"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor auto="true"/>
-        <bgColor auto="true"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor auto="true"/>
-        <bgColor auto="true"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor auto="true"/>
-        <bgColor auto="true"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor auto="true"/>
-        <bgColor auto="true"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor auto="true"/>
-        <bgColor auto="true"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor auto="true"/>
-        <bgColor auto="true"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor auto="true"/>
-        <bgColor auto="true"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor auto="true"/>
-        <bgColor auto="true"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor auto="true"/>
-        <bgColor auto="true"/>
+  <fills count="33">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -216,105 +497,312 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="8" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="6" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="22" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="2" fillId="3" fontId="0" numFmtId="22" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="3" fillId="4" fontId="0" numFmtId="22" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="4" fillId="5" fontId="0" numFmtId="22" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="5" fillId="6" fontId="0" numFmtId="22" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="6" fillId="7" fontId="0" numFmtId="22" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="7" fillId="8" fontId="0" numFmtId="22" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="8" fillId="9" fontId="0" numFmtId="22" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="9" fillId="10" fontId="0" numFmtId="22" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFill="true" applyFont="false" applyNumberFormat="true" applyProtection="false" borderId="10" fillId="11" fontId="0" numFmtId="22" xfId="0"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -363,7 +851,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -396,26 +884,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -448,23 +919,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -606,71 +1060,66 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" max="1" min="1" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" max="2" min="2" style="0" width="41.42578125"/>
-    <col bestFit="true" collapsed="false" customWidth="true" hidden="false" max="3" min="3" style="0" width="5.42578125"/>
-    <col bestFit="true" collapsed="false" customWidth="true" hidden="false" max="5" min="5" style="0" width="9.5703125"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="41.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="5.42857142857143" customWidth="1"/>
+    <col min="5" max="5" width="9.57142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4">
         <v>0</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>786936732658</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>12</v>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -682,12 +1131,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>725272730706</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>33</v>
@@ -699,12 +1148,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>28400589895</v>
       </c>
-      <c r="B5" t="str">
-        <v>Trucks_having_sex</v>
+      <c r="B5" t="s">
+        <v>8</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -716,12 +1165,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>13000006057</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -733,12 +1182,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>737452918903</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -754,8 +1203,8 @@
       <c r="A8">
         <v>674398202423</v>
       </c>
-      <c r="B8" t="str">
-        <v>Piano_Book</v>
+      <c r="B8" t="s">
+        <v>11</v>
       </c>
       <c r="C8">
         <v>15</v>
@@ -775,7 +1224,7 @@
         <v>490810512013</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -790,12 +1239,12 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>29000073692</v>
       </c>
-      <c r="B10" t="str">
-        <v>rrreee</v>
+      <c r="B10" t="s">
+        <v>13</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -807,12 +1256,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>888670109472</v>
       </c>
-      <c r="B11" t="str">
-        <v>Mixed_Nut_can_2</v>
+      <c r="B11" t="s">
+        <v>14</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -824,12 +1273,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>750515018013</v>
       </c>
-      <c r="B12" t="str">
-        <v>Cracker_Cart</v>
+      <c r="B12" t="s">
+        <v>15</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -841,12 +1290,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>16000179356</v>
       </c>
-      <c r="B13" t="str">
-        <v>Samus</v>
+      <c r="B13" t="s">
+        <v>16</v>
       </c>
       <c r="C13">
         <v>11</v>
@@ -858,12 +1307,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>44000010461</v>
       </c>
-      <c r="B14" t="str">
-        <v>rejlk</v>
+      <c r="B14" t="s">
+        <v>17</v>
       </c>
       <c r="C14">
         <v>19</v>
@@ -875,12 +1324,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>96619284108</v>
       </c>
-      <c r="B15" t="str">
-        <v>333</v>
+      <c r="B15" t="s">
+        <v>18</v>
       </c>
       <c r="C15">
         <v>222</v>
@@ -893,102 +1342,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C833EDD-534B-42B2-BDD2-559E8412576C}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>44503.804363425923</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5">
-        <v>44503.898853070074</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="6">
-        <v>44504.407790594174</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:G9"/>
-  <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col bestFit="true" collapsed="false" customWidth="true" hidden="false" max="1" min="1" style="0" width="12"/>
-    <col bestFit="true" collapsed="false" customWidth="true" hidden="false" max="2" min="2" style="0" width="11.42578125"/>
-    <col bestFit="true" collapsed="false" customWidth="true" hidden="false" max="5" min="5" style="0" width="9.7109375"/>
-    <col bestFit="true" collapsed="false" customWidth="true" hidden="false" max="6" min="6" style="0" width="9.5703125"/>
-    <col bestFit="true" collapsed="false" customWidth="true" hidden="false" max="7" min="7" style="0" width="9.7109375"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="11.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="9.71428571428571" customWidth="1"/>
+    <col min="6" max="6" width="9.57142857142857" customWidth="1"/>
+    <col min="7" max="7" width="9.71428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -996,22 +1370,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1019,7 +1393,7 @@
         <v>674398202423</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1034,7 +1408,7 @@
         <v>-2</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1042,7 +1416,7 @@
         <v>674398202423</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1054,7 +1428,7 @@
         <v>43</v>
       </c>
       <c r="G3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1062,7 +1436,7 @@
         <v>674398202423</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1077,7 +1451,7 @@
         <v>-2</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1085,7 +1459,7 @@
         <v>490810512013</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1100,7 +1474,7 @@
         <v>-1</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1108,7 +1482,7 @@
         <v>674398202423</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1123,7 +1497,7 @@
         <v>-4</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1131,7 +1505,7 @@
         <v>674398202423</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -1146,7 +1520,7 @@
         <v>-6</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1154,7 +1528,7 @@
         <v>674398202423</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1169,7 +1543,7 @@
         <v>-7</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1177,7 +1551,7 @@
         <v>490810512013</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1192,15 +1566,15 @@
         <v>-2</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>674398202423</v>
       </c>
-      <c r="B10" t="str">
-        <v>Piano_Book</v>
+      <c r="B10" t="s">
+        <v>11</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1214,16 +1588,16 @@
       <c r="F10">
         <v>-8</v>
       </c>
-      <c r="G10" t="str">
-        <v>2021/12/5</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>674398202423</v>
       </c>
-      <c r="B11" t="str">
-        <v>Piano_Book</v>
+      <c r="B11" t="s">
+        <v>11</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -1237,16 +1611,16 @@
       <c r="F11">
         <v>-11</v>
       </c>
-      <c r="G11" t="str">
-        <v>2021/12/6</v>
-      </c>
-    </row>
-    <row r="12">
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>674398202423</v>
       </c>
-      <c r="B12" t="str">
-        <v>Piano_Book</v>
+      <c r="B12" t="s">
+        <v>11</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1260,16 +1634,16 @@
       <c r="F12">
         <v>-13</v>
       </c>
-      <c r="G12" t="str">
-        <v>2021/12/30</v>
-      </c>
-    </row>
-    <row r="13">
+      <c r="G12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>674398202423</v>
       </c>
-      <c r="B13" t="str">
-        <v>Piano_Book</v>
+      <c r="B13" t="s">
+        <v>11</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1283,16 +1657,16 @@
       <c r="F13">
         <v>-14</v>
       </c>
-      <c r="G13" t="str">
-        <v>2021/12/30</v>
-      </c>
-    </row>
-    <row r="14">
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>490810512013</v>
       </c>
-      <c r="B14" t="str">
-        <v>verrr</v>
+      <c r="B14" t="s">
+        <v>12</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1306,51 +1680,53 @@
       <c r="F14">
         <v>-3</v>
       </c>
-      <c r="G14" t="str">
-        <v>2021/12/30</v>
+      <c r="G14" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA8E916-4F10-47C2-8648-0145CB92AFF8}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="7" outlineLevelCol="4"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>13000006057</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
+      <c r="B2" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1358,16 +1734,16 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="8">
-        <v>44525.719176438659</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="3">
+        <v>44525.7191764387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>13000006057</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1375,16 +1751,16 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="9">
-        <v>44525.719464839116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="3">
+        <v>44525.7194648391</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>13000006057</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1392,16 +1768,16 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" s="10">
-        <v>44525.719869876615</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="3">
+        <v>44525.7198698766</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>13000006057</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1409,16 +1785,16 @@
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" s="11">
-        <v>44525.722403845633</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="3">
+        <v>44525.7224038456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>13000006057</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6">
         <v>12</v>
@@ -1426,16 +1802,16 @@
       <c r="D6">
         <v>12</v>
       </c>
-      <c r="E6" s="12">
-        <v>44525.723437086286</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="3">
+        <v>44525.7234370863</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>13000006057</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -1443,16 +1819,16 @@
       <c r="D7">
         <v>2</v>
       </c>
-      <c r="E7" s="13">
-        <v>44526.419351564517</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="3">
+        <v>44526.4193515645</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>13000006057</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -1460,11 +1836,12 @@
       <c r="D8">
         <v>2</v>
       </c>
-      <c r="E8" s="14">
-        <v>44526.420547988018</v>
+      <c r="E8" s="3">
+        <v>44526.420547988</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>